<commit_message>
added TP, FP, FN
</commit_message>
<xml_diff>
--- a/PrecisionRecall.xlsx
+++ b/PrecisionRecall.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="18920" windowHeight="13100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="380" yWindow="1580" windowWidth="20940" windowHeight="13100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="31">
   <si>
     <t>Precision</t>
   </si>
@@ -80,12 +82,54 @@
   </si>
   <si>
     <t>SVM on Color Histogram Without Dynamics (100 Trials)</t>
+  </si>
+  <si>
+    <t>SVM on Color Histogram With Dynamics (100 Trials)</t>
+  </si>
+  <si>
+    <t>Training Error</t>
+  </si>
+  <si>
+    <t>Generalization Error</t>
+  </si>
+  <si>
+    <t>SVM (RBF)</t>
+  </si>
+  <si>
+    <t>SVM (Gaussian)</t>
+  </si>
+  <si>
+    <t>SVM (Polynomial 2)</t>
+  </si>
+  <si>
+    <t>SVM (Polynomial 3)</t>
+  </si>
+  <si>
+    <t>SVM (Linear)</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>SVM on Raw Data (100 Trials)</t>
+  </si>
+  <si>
+    <t>SVM on Clustered Color Barcode (100 Trials)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -137,8 +181,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +194,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,38 +473,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L21"/>
+  <dimension ref="B1:R21"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="N1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -486,72 +542,101 @@
       <c r="L3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>0.47389999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>0.29599999999999999</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>0.24410000000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>0.27279999999999999</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>0.34920000000000001</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>0.2671</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>0.29210000000000003</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="3">
         <v>0.30530000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>0.36770000000000003</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>0.42630000000000001</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>0.2366</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>0.31809999999999999</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>0.33839999999999998</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>0.39739999999999998</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <v>0.34179999999999999</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>0.43990000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -582,72 +667,101 @@
       <c r="L7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>0.41210000000000002</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>0.59119999999999995</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>0.3725</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>0.33760000000000001</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>0.4304</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>0.65110000000000001</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="3">
         <v>0.41670000000000001</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="3">
         <v>0.35289999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>0.39329999999999998</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>0.62980000000000003</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>0.34150000000000003</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>0.3659</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>0.43840000000000001</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>0.68479999999999996</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
         <v>0.35489999999999999</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="3">
         <v>0.40799999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -678,72 +792,101 @@
       <c r="L11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>0.46360000000000001</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>0.69689999999999996</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>0.48139999999999999</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>0.47170000000000001</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>0.49070000000000003</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <v>0.61480000000000001</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="3">
         <v>0.41099999999999998</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="3">
         <v>0.47799999999999998</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>0.45090000000000002</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>0.76239999999999997</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>0.49359999999999998</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>0.43980000000000002</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>0.45219999999999999</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>0.71389999999999998</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <v>0.44030000000000002</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="3">
         <v>0.43359999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -774,72 +917,101 @@
       <c r="L15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>0.41420000000000001</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>0.74160000000000004</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>0.51729999999999998</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>0.4824</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="3">
         <v>0.46260000000000001</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <v>0.77559999999999996</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="3">
         <v>0.43409999999999999</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="3">
         <v>0.49580000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>0.48230000000000001</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>0.80430000000000001</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <v>0.47939999999999999</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="3">
         <v>0.45650000000000002</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>0.4395</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <v>0.77690000000000003</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="3">
         <v>0.48349999999999999</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="3">
         <v>0.4829</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -870,75 +1042,105 @@
       <c r="L19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P19" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>0.46539999999999998</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>0.81879999999999997</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>0.50409999999999999</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>0.54869999999999997</v>
       </c>
       <c r="H20" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>0.4662</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="3">
         <v>0.8256</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="3">
         <v>0.51729999999999998</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="3">
         <v>0.53449999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>0.48070000000000002</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>0.7782</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>0.50860000000000005</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>0.51880000000000004</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="3">
         <v>0.4793</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="3">
         <v>0.8044</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="3">
         <v>0.50600000000000001</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="3">
         <v>0.54510000000000003</v>
       </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -948,41 +1150,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -1035,79 +1237,79 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>0.36940000000000001</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>0.76419999999999999</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>0.33339999999999997</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>0.3503</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>0.36</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>0.80510000000000004</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>0.4194</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="3">
         <v>0.31609999999999999</v>
       </c>
       <c r="N4" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>0.37990000000000002</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>0.78849999999999998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>0.30020000000000002</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>0.36680000000000001</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>0.41220000000000001</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>0.83689999999999998</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <v>0.29759999999999998</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>0.44669999999999999</v>
       </c>
       <c r="N5" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -1160,79 +1362,79 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>0.42380000000000001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>0.74239999999999995</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>0.42159999999999997</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>0.36120000000000002</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>0.42849999999999999</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>0.73570000000000002</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="3">
         <v>0.41020000000000001</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="3">
         <v>0.40300000000000002</v>
       </c>
       <c r="N8" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>0.43930000000000002</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="3">
         <v>0.70040000000000002</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>0.38</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>0.35959999999999998</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>0.44529999999999997</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>0.7339</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
         <v>0.40570000000000001</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="3">
         <v>0.41499999999999998</v>
       </c>
       <c r="N9" t="s">
         <v>0</v>
       </c>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -1285,79 +1487,79 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>0.50239999999999996</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="3">
         <v>0.81489999999999996</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>0.39679999999999999</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>0.48070000000000002</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>0.53820000000000001</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <v>0.81100000000000005</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="3">
         <v>0.41539999999999999</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="3">
         <v>0.51390000000000002</v>
       </c>
       <c r="N12" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>0.52439999999999998</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="3">
         <v>0.81759999999999999</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>0.44379999999999997</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>0.43880000000000002</v>
       </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>0.50419999999999998</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>0.75529999999999997</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <v>0.47449999999999998</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="3">
         <v>0.50600000000000001</v>
       </c>
       <c r="N13" t="s">
         <v>0</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -1410,79 +1612,95 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>0.41010000000000002</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>0.72899999999999998</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>0.36890000000000001</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>0.44479999999999997</v>
       </c>
       <c r="H16" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="3">
         <v>0.42299999999999999</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <v>0.74</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="3">
         <v>0.3473</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="3">
         <v>0.38800000000000001</v>
       </c>
       <c r="N16" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="O16" s="3">
+        <v>0.4143</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0.72640000000000005</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0.44479999999999997</v>
+      </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>0.4093</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>0.7712</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <v>0.3821</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="3">
         <v>0.40400000000000003</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>0.42059999999999997</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <v>0.78239999999999998</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="3">
         <v>0.33589999999999998</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L17" s="3">
         <v>0.36</v>
       </c>
       <c r="N17" t="s">
         <v>0</v>
       </c>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="O17" s="3">
+        <v>0.4148</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0.77880000000000005</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0.376</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0.39389999999999997</v>
+      </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
@@ -1535,79 +1753,95 @@
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>0.42459999999999998</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>0.79649999999999999</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>0.38429999999999997</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>0.59330000000000005</v>
       </c>
       <c r="H20" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>0.48070000000000002</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="3">
         <v>0.74770000000000003</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="3">
         <v>0.35510000000000003</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="3">
         <v>0.53610000000000002</v>
       </c>
       <c r="N20" t="s">
         <v>1</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="O20" s="3">
+        <v>0.4582</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0.78239999999999998</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.40189999999999998</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0.50890000000000002</v>
+      </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>0.46829999999999999</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>0.72009999999999996</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>0.40179999999999999</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>0.53469999999999995</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="3">
         <v>0.47499999999999998</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="3">
         <v>0.73819999999999997</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="3">
         <v>0.37509999999999999</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="3">
         <v>0.51990000000000003</v>
       </c>
       <c r="N21" t="s">
         <v>0</v>
       </c>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="O21" s="3">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0.71619999999999995</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0.41549999999999998</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0.51649999999999996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1621,36 +1855,428 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="6">
+        <f>14*K17</f>
+        <v>6.4147999999999996</v>
+      </c>
+      <c r="I17" s="6">
+        <f>14-H17</f>
+        <v>7.5852000000000004</v>
+      </c>
+      <c r="J17" s="6">
+        <f>H17/L17-H17</f>
+        <v>6.9772668058455114</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.4582</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" ref="H18:H20" si="0">14*K18</f>
+        <v>10.9536</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" ref="I18:I20" si="1">14-H18</f>
+        <v>3.0464000000000002</v>
+      </c>
+      <c r="J18" s="6">
+        <f>H18/L18-H18</f>
+        <v>4.3404519407986601</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.78239999999999998</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.71619999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>5.6265999999999998</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="1"/>
+        <v>8.3734000000000002</v>
+      </c>
+      <c r="J19" s="6">
+        <f>H19/L19-H19</f>
+        <v>7.9151569193742475</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.40189999999999998</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.41549999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>7.1246</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="1"/>
+        <v>6.8754</v>
+      </c>
+      <c r="J20" s="6">
+        <f>H20/L20-H20</f>
+        <v>6.6693980638915784</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.50890000000000002</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.51649999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="6">
+        <v>6.1520000000000001</v>
+      </c>
+      <c r="C24" s="6">
+        <v>7.8479999999999999</v>
+      </c>
+      <c r="D24" s="6">
+        <v>7.8520000000000003</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.442</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.44180000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6">
+        <v>10.569000000000001</v>
+      </c>
+      <c r="C25" s="6">
+        <v>3.431</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2.9649999999999999</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.78239999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.5910000000000002</v>
+      </c>
+      <c r="C26" s="6">
+        <v>7.4089999999999998</v>
+      </c>
+      <c r="D26" s="6">
+        <v>7.1870000000000003</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.47410000000000002</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.48309999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6">
+        <v>6.601</v>
+      </c>
+      <c r="C27" s="6">
+        <v>7.399</v>
+      </c>
+      <c r="D27" s="6">
+        <v>8.0830000000000002</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.47439999999999999</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.45079999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A22:F22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="M14" sqref="M11:M14"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -1688,31 +2314,31 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.29170000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.2848</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>0.1971</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.32879999999999998</v>
       </c>
       <c r="H4" t="s">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0.25640000000000002</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>0.26690000000000003</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>0.27110000000000001</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>0.214</v>
       </c>
     </row>
@@ -1720,31 +2346,31 @@
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.3019</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>0.26240000000000002</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>0.249</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>0.26690000000000003</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>0.25340000000000001</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>0.29110000000000003</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>0.24099999999999999</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>0.2374</v>
       </c>
     </row>
@@ -1784,33 +2410,65 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="C8" s="3">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.25130000000000002</v>
+      </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="I8" s="3">
+        <v>0.26929999999999998</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.20230000000000001</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.26529999999999998</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.32890000000000003</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="C9" s="3">
+        <v>0.2717</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.2697</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.2457</v>
+      </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="I9" s="3">
+        <v>0.30420000000000003</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.21460000000000001</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.28460000000000002</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -1848,33 +2506,65 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="3">
+        <v>0.35060000000000002</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.2606</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.253</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.25540000000000002</v>
+      </c>
       <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="I12" s="3">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.27529999999999999</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.1426</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.22339999999999999</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="3">
+        <v>0.27939999999999998</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.31719999999999998</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.25069999999999998</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.26240000000000002</v>
+      </c>
       <c r="H13" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="I13" s="3">
+        <v>0.28360000000000002</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.26050000000000001</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.19359999999999999</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.22420000000000001</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -1912,33 +2602,65 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="C16" s="3">
+        <v>0.26860000000000001</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.32290000000000002</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.20549999999999999</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.27429999999999999</v>
+      </c>
       <c r="H16" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="I16" s="3">
+        <v>0.2412</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.33260000000000001</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.24529999999999999</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.2233</v>
+      </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="C17" s="3">
+        <v>0.2596</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.3266</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.22489999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.25380000000000003</v>
+      </c>
       <c r="H17" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="I17" s="3">
+        <v>0.22289999999999999</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.3276</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.23730000000000001</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.24349999999999999</v>
+      </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
@@ -1976,33 +2698,65 @@
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="C20" s="3">
+        <v>0.21510000000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.2944</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.27979999999999999</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.2389</v>
+      </c>
       <c r="H20" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="I20" s="3">
+        <v>0.18529999999999999</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.22339999999999999</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.31480000000000002</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.24679999999999999</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="C21" s="3">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.2611</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.30049999999999999</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.23499999999999999</v>
+      </c>
       <c r="H21" t="s">
         <v>0</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="I21" s="3">
+        <v>0.18279999999999999</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.3049</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.2702</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2011,4 +2765,79 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.61509999999999998</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.80359999999999998</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.82140000000000002</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.69640000000000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.28570000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>